<commit_message>
edito excel con mis resultados
</commit_message>
<xml_diff>
--- a/Entrega4/Resultados Consultas.xlsx
+++ b/Entrega4/Resultados Consultas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macar\Desktop\BBDD\Bases-de-Datos-IIC2413-2020-2\Entrega4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c07dd3d61be084f/Documentos/Universidad_OneDrive/2020-2/bdd/Bases-de-Datos-IIC2413-2020-2/Entrega4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650B54A1-2997-44C5-8748-166A589BEC36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{650B54A1-2997-44C5-8748-166A589BEC36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE55CFB4-4475-4FF4-8A78-E1C54230AB5E}"/>
   <bookViews>
-    <workbookView xWindow="13416" yWindow="7908" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>Consulta</t>
   </si>
@@ -276,12 +276,15 @@
   <si>
     <t>[]</t>
   </si>
+  <si>
+    <t>a mi m corre bien este me retorna todos lo smensajes eso si</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -333,6 +336,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -408,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -468,6 +478,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -690,23 +706,23 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H8" sqref="H8"/>
+      <selection pane="topRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="1"/>
-    <col min="2" max="2" width="50.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.44140625" style="1"/>
+    <col min="1" max="1" width="14.453125" style="1"/>
+    <col min="2" max="2" width="50.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -726,7 +742,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -746,7 +762,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -765,8 +781,11 @@
       <c r="F3" s="16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G3" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -786,7 +805,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -804,7 +823,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -823,8 +842,11 @@
       <c r="F6" s="16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G6" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -844,7 +866,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -862,7 +884,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
@@ -881,8 +903,11 @@
       <c r="F9" s="16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G9" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="63" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>27</v>
       </c>
@@ -901,8 +926,11 @@
       <c r="F10" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G10" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>29</v>
       </c>
@@ -921,8 +949,9 @@
       <c r="F11" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>32</v>
       </c>
@@ -941,7 +970,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
@@ -961,7 +990,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>39</v>
       </c>
@@ -981,7 +1010,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>43</v>
       </c>
@@ -999,7 +1028,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>46</v>
       </c>
@@ -1017,7 +1046,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>48</v>
       </c>
@@ -1035,7 +1064,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>51</v>
       </c>
@@ -1053,7 +1082,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>53</v>
       </c>
@@ -1073,7 +1102,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -1091,7 +1120,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
@@ -1111,7 +1140,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>62</v>
       </c>
@@ -1131,7 +1160,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>65</v>
       </c>
@@ -1151,7 +1180,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>68</v>
       </c>

</xml_diff>